<commit_message>
TRANSLATE-547: Filesize of generated Excel-Statistics is to big
</commit_message>
<xml_diff>
--- a/application/modules/editor/Plugins/SegmentStatistics/templates/export-template.xlsx
+++ b/application/modules/editor/Plugins/SegmentStatistics/templates/export-template.xlsx
@@ -184,83 +184,82 @@
     <t>Termini formal inkorrekt</t>
   </si>
   <si>
+    <t>Häufigkeit korrekt</t>
+  </si>
+  <si>
+    <t>Häufigkeit inkorrekt</t>
+  </si>
+  <si>
+    <t>Erklärungen</t>
+  </si>
+  <si>
+    <t>Statusoptionen:</t>
+  </si>
+  <si>
+    <t>(1) Änderung durchgeführt</t>
+  </si>
+  <si>
+    <t>(2) Neue VZB nicht passend</t>
+  </si>
+  <si>
+    <t>(3) Zielterm nicht vorhanden</t>
+  </si>
+  <si>
+    <t>(4) Keine Änderung nötig</t>
+  </si>
+  <si>
+    <t>(5) Quell-/Zielsegment nicht passend</t>
+  </si>
+  <si>
+    <t>(6) Nacharbeit</t>
+  </si>
+  <si>
+    <t>Termini Status X: Anzahl der Termini in Segmenten, die den Status X haben (gezählt werden für den roten Block die rot markierten Termini, für den blauen Block die blau markierten)</t>
+  </si>
+  <si>
+    <t>Zeichen: werden immer im Target (Zielsprache) gezählt</t>
+  </si>
+  <si>
+    <t>Zeilen: Berechnung: Zeichen / 55</t>
+  </si>
+  <si>
+    <t>Termini im blauen Block: Termini im Source (Quellsprache) mit Entsprechung im Target (Zielsprache), im Editor blau markiert ( = termFound im source)</t>
+  </si>
+  <si>
+    <t>Segmente im roten Block: Segmente im Source (Quellsprache) mit mindestens einem rot markierten Terminus. Im Editor sind das zum Zeitpunkt des Imports alle nicht gesperrten Segmente (= segmentsNotFound im source)</t>
+  </si>
+  <si>
+    <t>Segmente im blauen Block: Segmente im Source (Quellsprache) mit mindestens einem blau markierten Terminus. Im Editor sind das alle gesperrten Segmente und ein Teil der nicht gesperrten (= segmentsFound im source)</t>
+  </si>
+  <si>
+    <t>Wörter im roten Block: Anzahl der Wörter in Segmenten mit mindestens einem rot markierten Terminus</t>
+  </si>
+  <si>
+    <t>Wörter im blauen Block: Anzahl der Wörter in Segmenten mit mindestens einem blau markierten Terminus</t>
+  </si>
+  <si>
+    <t>Die Arbeitsblätter 3 bis n sind nach den Zeilen auf dem Blatt „Zusammenfassung“ benannt.</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Terminus </t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="10"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <rFont val="Arial"/>
         <family val="2"/>
-        <scheme val="minor"/>
       </rPr>
-      <t>[nach Häufigkeit korrekt geordnet]</t>
+      <t xml:space="preserve">[nach Häufigkeit korrekt geordnet] </t>
     </r>
-  </si>
-  <si>
-    <t>Häufigkeit korrekt</t>
-  </si>
-  <si>
-    <t>Häufigkeit inkorrekt</t>
-  </si>
-  <si>
-    <t>Erklärungen</t>
-  </si>
-  <si>
-    <t>Statusoptionen:</t>
-  </si>
-  <si>
-    <t>(1) Änderung durchgeführt</t>
-  </si>
-  <si>
-    <t>(2) Neue VZB nicht passend</t>
-  </si>
-  <si>
-    <t>(3) Zielterm nicht vorhanden</t>
-  </si>
-  <si>
-    <t>(4) Keine Änderung nötig</t>
-  </si>
-  <si>
-    <t>(5) Quell-/Zielsegment nicht passend</t>
-  </si>
-  <si>
-    <t>(6) Nacharbeit</t>
-  </si>
-  <si>
-    <t>Termini Status X: Anzahl der Termini in Segmenten, die den Status X haben (gezählt werden für den roten Block die rot markierten Termini, für den blauen Block die blau markierten)</t>
-  </si>
-  <si>
-    <t>Zeichen: werden immer im Target (Zielsprache) gezählt</t>
-  </si>
-  <si>
-    <t>Zeilen: Berechnung: Zeichen / 55</t>
-  </si>
-  <si>
-    <t>Termini im blauen Block: Termini im Source (Quellsprache) mit Entsprechung im Target (Zielsprache), im Editor blau markiert ( = termFound im source)</t>
-  </si>
-  <si>
-    <t>Segmente im roten Block: Segmente im Source (Quellsprache) mit mindestens einem rot markierten Terminus. Im Editor sind das zum Zeitpunkt des Imports alle nicht gesperrten Segmente (= segmentsNotFound im source)</t>
-  </si>
-  <si>
-    <t>Segmente im blauen Block: Segmente im Source (Quellsprache) mit mindestens einem blau markierten Terminus. Im Editor sind das alle gesperrten Segmente und ein Teil der nicht gesperrten (= segmentsFound im source)</t>
-  </si>
-  <si>
-    <t>Wörter im roten Block: Anzahl der Wörter in Segmenten mit mindestens einem rot markierten Terminus</t>
-  </si>
-  <si>
-    <t>Wörter im blauen Block: Anzahl der Wörter in Segmenten mit mindestens einem blau markierten Terminus</t>
-  </si>
-  <si>
-    <t>Die Arbeitsblätter 3 bis n sind nach den Zeilen auf dem Blatt „Zusammenfassung“ benannt.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -325,10 +324,56 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF666666"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -390,37 +435,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -447,24 +468,46 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -762,816 +805,818 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BB7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="60.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:54">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="3" t="s">
+      <c r="C1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="4" t="s">
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31"/>
+      <c r="R1" s="31"/>
+      <c r="S1" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4"/>
-      <c r="AD1" s="4"/>
-      <c r="AE1" s="4"/>
-      <c r="AF1" s="4"/>
-      <c r="AG1" s="5" t="s">
+      <c r="T1" s="32"/>
+      <c r="U1" s="32"/>
+      <c r="V1" s="32"/>
+      <c r="W1" s="32"/>
+      <c r="X1" s="32"/>
+      <c r="Y1" s="32"/>
+      <c r="Z1" s="32"/>
+      <c r="AA1" s="32"/>
+      <c r="AB1" s="32"/>
+      <c r="AC1" s="32"/>
+      <c r="AD1" s="32"/>
+      <c r="AE1" s="32"/>
+      <c r="AF1" s="32"/>
+      <c r="AG1" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="AH1" s="5"/>
-      <c r="AI1" s="5"/>
-      <c r="AJ1" s="5"/>
-      <c r="AK1" s="5"/>
-      <c r="AL1" s="5"/>
-      <c r="AM1" s="5"/>
-      <c r="AN1" s="5"/>
-      <c r="AO1" s="5"/>
-      <c r="AP1" s="5"/>
-      <c r="AQ1" s="5"/>
-      <c r="AR1" s="5"/>
-      <c r="AS1" s="6"/>
-      <c r="AT1" s="6"/>
-      <c r="AU1" s="7" t="s">
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="33"/>
+      <c r="AJ1" s="33"/>
+      <c r="AK1" s="33"/>
+      <c r="AL1" s="33"/>
+      <c r="AM1" s="33"/>
+      <c r="AN1" s="33"/>
+      <c r="AO1" s="33"/>
+      <c r="AP1" s="33"/>
+      <c r="AQ1" s="33"/>
+      <c r="AR1" s="33"/>
+      <c r="AS1" s="2"/>
+      <c r="AT1" s="2"/>
+      <c r="AU1" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="AV1" s="7"/>
-      <c r="AW1" s="7"/>
-      <c r="AX1" s="7"/>
-      <c r="AY1" s="7"/>
-      <c r="AZ1" s="7"/>
-      <c r="BA1" s="7"/>
-      <c r="BB1" s="7"/>
-    </row>
-    <row r="2" spans="1:54" ht="26.25">
-      <c r="A2" s="1" t="s">
+      <c r="AV1" s="34"/>
+      <c r="AW1" s="34"/>
+      <c r="AX1" s="34"/>
+      <c r="AY1" s="34"/>
+      <c r="AZ1" s="34"/>
+      <c r="BA1" s="34"/>
+      <c r="BB1" s="34"/>
+    </row>
+    <row r="2" spans="1:54" s="22" customFormat="1" ht="25.5">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="O2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="P2" s="9" t="s">
+      <c r="P2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" s="8" t="s">
+      <c r="Q2" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="9" t="s">
+      <c r="R2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="8" t="s">
+      <c r="S2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="T2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U2" s="8" t="s">
+      <c r="U2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="V2" s="8" t="s">
+      <c r="V2" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="W2" s="8" t="s">
+      <c r="W2" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="X2" s="8" t="s">
+      <c r="X2" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="Y2" s="8" t="s">
+      <c r="Y2" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="Z2" s="8" t="s">
+      <c r="Z2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="AA2" s="8" t="s">
+      <c r="AA2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="AB2" s="8" t="s">
+      <c r="AB2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="AC2" s="9" t="s">
+      <c r="AC2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AD2" s="9" t="s">
+      <c r="AD2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AE2" s="8" t="s">
+      <c r="AE2" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="AF2" s="9" t="s">
+      <c r="AF2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AG2" s="8" t="s">
+      <c r="AG2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="AH2" s="9" t="s">
+      <c r="AH2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="AI2" s="8" t="s">
+      <c r="AI2" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="AJ2" s="8" t="s">
+      <c r="AJ2" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="AK2" s="8" t="s">
+      <c r="AK2" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="AL2" s="8" t="s">
+      <c r="AL2" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="AM2" s="8" t="s">
+      <c r="AM2" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="AN2" s="8" t="s">
+      <c r="AN2" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="AO2" s="8" t="s">
+      <c r="AO2" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="AP2" s="8" t="s">
+      <c r="AP2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="AQ2" s="9" t="s">
+      <c r="AQ2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AR2" s="9" t="s">
+      <c r="AR2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AS2" s="8" t="s">
+      <c r="AS2" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="AT2" s="9" t="s">
+      <c r="AT2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AU2" s="9" t="s">
+      <c r="AU2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AV2" s="9" t="s">
+      <c r="AV2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="AW2" s="9" t="s">
+      <c r="AW2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AX2" s="9" t="s">
+      <c r="AX2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="AY2" s="9" t="s">
+      <c r="AY2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AZ2" s="9" t="s">
+      <c r="AZ2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="BA2" s="9" t="s">
+      <c r="BA2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="BB2" s="9" t="s">
+      <c r="BB2" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="25" customFormat="1">
-      <c r="A3" s="22" t="s">
+    <row r="3" spans="1:54" s="19" customFormat="1" ht="12.75">
+      <c r="A3" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="23" t="e">
+      <c r="D3" s="16" t="e">
         <f>ROUND(C3/55,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="23" t="e">
+      <c r="G3" s="16" t="e">
         <f>ROUND(E3/D3, 2)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="H3" s="23" t="e">
+      <c r="H3" s="16" t="e">
         <f>ROUND(E3/F3, 2)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="I3" s="24" t="s">
+      <c r="I3" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="23" t="e">
+      <c r="J3" s="16" t="e">
         <f>ROUND(I3/F3,2)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="K3" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="23" t="e">
+      <c r="L3" s="16" t="e">
         <f>ROUND(K3/55,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M3" s="22" t="s">
+      <c r="M3" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="22" t="s">
+      <c r="N3" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="O3" s="23" t="e">
+      <c r="O3" s="16" t="e">
         <f>ROUND(M3/L3, 2)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="P3" s="23" t="e">
+      <c r="P3" s="16" t="e">
         <f>ROUND(M3/N3, 2)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="Q3" s="22" t="s">
+      <c r="Q3" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="R3" s="23" t="e">
+      <c r="R3" s="16" t="e">
         <f>ROUND(Q3/N3,2)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="S3" s="22" t="s">
+      <c r="S3" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="T3" s="23" t="e">
+      <c r="T3" s="16" t="e">
         <f>ROUND(S3/55,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="U3" s="22" t="s">
+      <c r="U3" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="V3" s="24" t="s">
+      <c r="V3" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="W3" s="24" t="s">
+      <c r="W3" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="X3" s="24" t="s">
+      <c r="X3" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="Y3" s="24" t="s">
+      <c r="Y3" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="Z3" s="24" t="s">
+      <c r="Z3" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="AA3" s="24" t="s">
+      <c r="AA3" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="AB3" s="22" t="s">
+      <c r="AB3" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="AC3" s="23" t="e">
+      <c r="AC3" s="16" t="e">
         <f>ROUND(U3/T3, 2)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AD3" s="23" t="e">
+      <c r="AD3" s="16" t="e">
         <f>ROUND(U3/AB3, 2)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AE3" s="24" t="s">
+      <c r="AE3" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="AF3" s="23" t="e">
+      <c r="AF3" s="16" t="e">
         <f>ROUND(AE3/AB3,2)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AG3" s="22" t="s">
+      <c r="AG3" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="AH3" s="23" t="e">
+      <c r="AH3" s="16" t="e">
         <f>ROUND(AG3/55,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AI3" s="22" t="s">
+      <c r="AI3" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="AJ3" s="24" t="s">
+      <c r="AJ3" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="AK3" s="24" t="s">
+      <c r="AK3" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="AL3" s="24" t="s">
+      <c r="AL3" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="AM3" s="24" t="s">
+      <c r="AM3" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="AN3" s="24" t="s">
+      <c r="AN3" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="AO3" s="24" t="s">
+      <c r="AO3" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="AP3" s="22" t="s">
+      <c r="AP3" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="AQ3" s="23" t="e">
+      <c r="AQ3" s="16" t="e">
         <f>ROUND(AI3/AH3, 2)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AR3" s="23" t="e">
+      <c r="AR3" s="16" t="e">
         <f>ROUND(AI3/AP3, 2)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AS3" s="24" t="s">
+      <c r="AS3" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="AT3" s="23" t="e">
+      <c r="AT3" s="16" t="e">
         <f>ROUND(AS3/AP3,2)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AU3" s="23" t="e">
+      <c r="AU3" s="16" t="e">
         <f>C3-S3</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AV3" s="23" t="e">
+      <c r="AV3" s="16" t="e">
         <f>D3-T3</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AW3" s="23" t="e">
+      <c r="AW3" s="16" t="e">
         <f>E3-U3</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AX3" s="23" t="e">
+      <c r="AX3" s="16" t="e">
         <f>F3-AB3</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AY3" s="23" t="e">
+      <c r="AY3" s="16" t="e">
         <f>ROUND(AW3/AV3, 2)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AZ3" s="23" t="e">
+      <c r="AZ3" s="16" t="e">
         <f>ROUND(AW3/AX3, 2)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BA3" s="23" t="e">
+      <c r="BA3" s="16" t="e">
         <f>I3-AE3</f>
         <v>#VALUE!</v>
       </c>
-      <c r="BB3" s="23" t="e">
+      <c r="BB3" s="16" t="e">
         <f>BA3/AX3</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="4" spans="1:54">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:54" s="22" customFormat="1" ht="12.75">
+      <c r="A4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="4">
         <f>SUM(B3:B3)</f>
         <v>0</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="4">
         <f>SUM(C3:C3)</f>
         <v>0</v>
       </c>
-      <c r="D4" s="11" t="e">
+      <c r="D4" s="3" t="e">
         <f>SUM(D3:D3)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="4">
         <f>SUM(E3:E3)</f>
         <v>0</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="4">
         <f>SUM(F3:F3)</f>
         <v>0</v>
       </c>
-      <c r="G4" s="11" t="e">
+      <c r="G4" s="3" t="e">
         <f>ROUND(E4/D4, 2)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="H4" s="11" t="e">
+      <c r="H4" s="3" t="e">
         <f t="shared" ref="H4" si="0">ROUND(E4/F4, 2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="4">
         <f>SUM(I3:I3)</f>
         <v>0</v>
       </c>
-      <c r="J4" s="11" t="e">
+      <c r="J4" s="3" t="e">
         <f>ROUND(I4/F4,2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="4">
         <f>SUM(K3:K3)</f>
         <v>0</v>
       </c>
-      <c r="L4" s="1" t="e">
+      <c r="L4" s="4" t="e">
         <f>SUM(L3:L3)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="M4" s="1">
+      <c r="M4" s="4">
         <f>SUM(M3:M3)</f>
         <v>0</v>
       </c>
-      <c r="N4" s="1">
+      <c r="N4" s="4">
         <f>SUM(N3:N3)</f>
         <v>0</v>
       </c>
-      <c r="O4" s="11" t="e">
+      <c r="O4" s="3" t="e">
         <f>ROUND(M4/L4, 2)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="P4" s="11" t="e">
+      <c r="P4" s="3" t="e">
         <f t="shared" ref="P4" si="1">ROUND(M4/N4, 2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q4" s="1">
+      <c r="Q4" s="4">
         <f>SUM(Q3:Q3)</f>
         <v>0</v>
       </c>
-      <c r="R4" s="10" t="e">
+      <c r="R4" s="3" t="e">
         <f>ROUND(Q4/N4,2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="S4" s="1">
+      <c r="S4" s="4">
         <f t="shared" ref="S4:AB4" si="2">SUM(S3:S3)</f>
         <v>0</v>
       </c>
-      <c r="T4" s="1" t="e">
+      <c r="T4" s="4" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
-      <c r="U4" s="1">
+      <c r="U4" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="V4" s="1">
+      <c r="V4" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="W4" s="1">
+      <c r="W4" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X4" s="1">
+      <c r="X4" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y4" s="1">
+      <c r="Y4" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Z4" s="1">
+      <c r="Z4" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA4" s="1">
+      <c r="AA4" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AB4" s="1">
+      <c r="AB4" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC4" s="10" t="e">
+      <c r="AC4" s="3" t="e">
         <f>ROUND(U4/T4, 2)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AD4" s="10" t="e">
+      <c r="AD4" s="3" t="e">
         <f>ROUND(U4/AB4, 2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AE4" s="1">
+      <c r="AE4" s="4">
         <f>SUM(AE3:AE3)</f>
         <v>0</v>
       </c>
-      <c r="AF4" s="10" t="e">
+      <c r="AF4" s="3" t="e">
         <f>ROUND(AE4/AB4,2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AG4" s="1">
+      <c r="AG4" s="4">
         <f t="shared" ref="AG4:AP4" si="3">SUM(AG3:AG3)</f>
         <v>0</v>
       </c>
-      <c r="AH4" s="1" t="e">
+      <c r="AH4" s="4" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AI4" s="1">
+      <c r="AI4" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AJ4" s="1">
+      <c r="AJ4" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AK4" s="1">
+      <c r="AK4" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AL4" s="1">
+      <c r="AL4" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AM4" s="1">
+      <c r="AM4" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AN4" s="1">
+      <c r="AN4" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AO4" s="1">
+      <c r="AO4" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AP4" s="1">
+      <c r="AP4" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AQ4" s="11" t="e">
+      <c r="AQ4" s="3" t="e">
         <f>ROUND(AI4/AH4, 2)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AR4" s="11" t="e">
+      <c r="AR4" s="3" t="e">
         <f>ROUND(AI4/AP4, 2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AS4" s="1">
+      <c r="AS4" s="4">
         <f>SUM(AS3:AS3)</f>
         <v>0</v>
       </c>
-      <c r="AT4" s="10" t="e">
+      <c r="AT4" s="3" t="e">
         <f>ROUND(AS4/AP4,2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AU4" s="1" t="e">
+      <c r="AU4" s="4" t="e">
         <f t="shared" ref="AU4:BB4" si="4">SUM(AU3:AU3)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="AV4" s="1" t="e">
+      <c r="AV4" s="4" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AW4" s="1" t="e">
+      <c r="AW4" s="4" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AX4" s="1" t="e">
+      <c r="AX4" s="4" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AY4" s="1" t="e">
+      <c r="AY4" s="4" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="AZ4" s="1" t="e">
+      <c r="AZ4" s="4" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="BA4" s="1" t="e">
+      <c r="BA4" s="4" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="BB4" s="1" t="e">
+      <c r="BB4" s="4" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="5" spans="1:54">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="16"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="18"/>
-      <c r="T5" s="19"/>
-      <c r="U5" s="18"/>
-      <c r="V5" s="18"/>
-      <c r="W5" s="18"/>
-      <c r="X5" s="18"/>
-      <c r="Y5" s="18"/>
-      <c r="Z5" s="18"/>
-      <c r="AA5" s="18"/>
-      <c r="AB5" s="18"/>
-      <c r="AC5" s="19"/>
-      <c r="AD5" s="18"/>
-      <c r="AE5" s="18"/>
-      <c r="AF5" s="18"/>
-      <c r="AG5" s="20"/>
-      <c r="AH5" s="19"/>
-      <c r="AI5" s="20"/>
-      <c r="AJ5" s="20"/>
-      <c r="AK5" s="20"/>
-      <c r="AL5" s="20"/>
-      <c r="AM5" s="20"/>
-      <c r="AN5" s="20"/>
-      <c r="AO5" s="20"/>
-      <c r="AP5" s="20"/>
-      <c r="AQ5" s="19"/>
-      <c r="AR5" s="18"/>
-      <c r="AS5" s="18"/>
-      <c r="AT5" s="18"/>
-      <c r="AU5" s="20"/>
-      <c r="AV5" s="19"/>
-      <c r="AW5" s="20"/>
-      <c r="AX5" s="20"/>
-      <c r="AY5" s="19"/>
-      <c r="AZ5" s="19"/>
-      <c r="BA5" s="19"/>
-      <c r="BB5" s="17"/>
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="10"/>
+      <c r="AA5" s="10"/>
+      <c r="AB5" s="10"/>
+      <c r="AC5" s="11"/>
+      <c r="AD5" s="10"/>
+      <c r="AE5" s="10"/>
+      <c r="AF5" s="10"/>
+      <c r="AG5" s="12"/>
+      <c r="AH5" s="11"/>
+      <c r="AI5" s="12"/>
+      <c r="AJ5" s="12"/>
+      <c r="AK5" s="12"/>
+      <c r="AL5" s="12"/>
+      <c r="AM5" s="12"/>
+      <c r="AN5" s="12"/>
+      <c r="AO5" s="12"/>
+      <c r="AP5" s="12"/>
+      <c r="AQ5" s="11"/>
+      <c r="AR5" s="10"/>
+      <c r="AS5" s="10"/>
+      <c r="AT5" s="10"/>
+      <c r="AU5" s="12"/>
+      <c r="AV5" s="11"/>
+      <c r="AW5" s="12"/>
+      <c r="AX5" s="12"/>
+      <c r="AY5" s="11"/>
+      <c r="AZ5" s="11"/>
+      <c r="BA5" s="11"/>
+      <c r="BB5" s="9"/>
     </row>
     <row r="6" spans="1:54">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="17"/>
-      <c r="S6" s="18"/>
-      <c r="T6" s="19"/>
-      <c r="U6" s="18"/>
-      <c r="V6" s="18"/>
-      <c r="W6" s="18"/>
-      <c r="X6" s="18"/>
-      <c r="Y6" s="18"/>
-      <c r="Z6" s="18"/>
-      <c r="AA6" s="18"/>
-      <c r="AB6" s="18"/>
-      <c r="AC6" s="19"/>
-      <c r="AD6" s="18"/>
-      <c r="AE6" s="18"/>
-      <c r="AF6" s="18"/>
-      <c r="AG6" s="20"/>
-      <c r="AH6" s="19"/>
-      <c r="AI6" s="20"/>
-      <c r="AJ6" s="20"/>
-      <c r="AK6" s="20"/>
-      <c r="AL6" s="20"/>
-      <c r="AM6" s="20"/>
-      <c r="AN6" s="20"/>
-      <c r="AO6" s="20"/>
-      <c r="AP6" s="20"/>
-      <c r="AQ6" s="19"/>
-      <c r="AR6" s="18"/>
-      <c r="AS6" s="18"/>
-      <c r="AT6" s="18"/>
-      <c r="AU6" s="20"/>
-      <c r="AV6" s="19"/>
-      <c r="AW6" s="20"/>
-      <c r="AX6" s="20"/>
-      <c r="AY6" s="19"/>
-      <c r="AZ6" s="19"/>
-      <c r="BA6" s="19"/>
-      <c r="BB6" s="17"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="11"/>
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="10"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="10"/>
+      <c r="AA6" s="10"/>
+      <c r="AB6" s="10"/>
+      <c r="AC6" s="11"/>
+      <c r="AD6" s="10"/>
+      <c r="AE6" s="10"/>
+      <c r="AF6" s="10"/>
+      <c r="AG6" s="12"/>
+      <c r="AH6" s="11"/>
+      <c r="AI6" s="12"/>
+      <c r="AJ6" s="12"/>
+      <c r="AK6" s="12"/>
+      <c r="AL6" s="12"/>
+      <c r="AM6" s="12"/>
+      <c r="AN6" s="12"/>
+      <c r="AO6" s="12"/>
+      <c r="AP6" s="12"/>
+      <c r="AQ6" s="11"/>
+      <c r="AR6" s="10"/>
+      <c r="AS6" s="10"/>
+      <c r="AT6" s="10"/>
+      <c r="AU6" s="12"/>
+      <c r="AV6" s="11"/>
+      <c r="AW6" s="12"/>
+      <c r="AX6" s="12"/>
+      <c r="AY6" s="11"/>
+      <c r="AZ6" s="11"/>
+      <c r="BA6" s="11"/>
+      <c r="BB6" s="9"/>
     </row>
     <row r="7" spans="1:54">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="17"/>
-      <c r="Q7" s="17"/>
-      <c r="R7" s="17"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="19"/>
-      <c r="U7" s="18"/>
-      <c r="V7" s="18"/>
-      <c r="W7" s="18"/>
-      <c r="X7" s="18"/>
-      <c r="Y7" s="18"/>
-      <c r="Z7" s="18"/>
-      <c r="AA7" s="18"/>
-      <c r="AB7" s="18"/>
-      <c r="AC7" s="19"/>
-      <c r="AD7" s="18"/>
-      <c r="AE7" s="18"/>
-      <c r="AF7" s="18"/>
-      <c r="AG7" s="20"/>
-      <c r="AH7" s="19"/>
-      <c r="AI7" s="20"/>
-      <c r="AJ7" s="20"/>
-      <c r="AK7" s="20"/>
-      <c r="AL7" s="20"/>
-      <c r="AM7" s="20"/>
-      <c r="AN7" s="20"/>
-      <c r="AO7" s="20"/>
-      <c r="AP7" s="20"/>
-      <c r="AQ7" s="19"/>
-      <c r="AR7" s="18"/>
-      <c r="AS7" s="18"/>
-      <c r="AT7" s="18"/>
-      <c r="AU7" s="20"/>
-      <c r="AV7" s="19"/>
-      <c r="AW7" s="20"/>
-      <c r="AX7" s="20"/>
-      <c r="AY7" s="19"/>
-      <c r="AZ7" s="19"/>
-      <c r="BA7" s="19"/>
-      <c r="BB7" s="17"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="9"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="11"/>
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="10"/>
+      <c r="AA7" s="10"/>
+      <c r="AB7" s="10"/>
+      <c r="AC7" s="11"/>
+      <c r="AD7" s="10"/>
+      <c r="AE7" s="10"/>
+      <c r="AF7" s="10"/>
+      <c r="AG7" s="12"/>
+      <c r="AH7" s="11"/>
+      <c r="AI7" s="12"/>
+      <c r="AJ7" s="12"/>
+      <c r="AK7" s="12"/>
+      <c r="AL7" s="12"/>
+      <c r="AM7" s="12"/>
+      <c r="AN7" s="12"/>
+      <c r="AO7" s="12"/>
+      <c r="AP7" s="12"/>
+      <c r="AQ7" s="11"/>
+      <c r="AR7" s="10"/>
+      <c r="AS7" s="10"/>
+      <c r="AT7" s="10"/>
+      <c r="AU7" s="12"/>
+      <c r="AV7" s="11"/>
+      <c r="AW7" s="12"/>
+      <c r="AX7" s="12"/>
+      <c r="AY7" s="11"/>
+      <c r="AZ7" s="11"/>
+      <c r="BA7" s="11"/>
+      <c r="BB7" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -1590,55 +1635,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="74.140625" customWidth="1"/>
-    <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1"/>
+    <col min="1" max="1" width="70.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:3" s="24" customFormat="1">
+      <c r="A1" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="26" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+    </row>
+    <row r="2" spans="1:3" s="24" customFormat="1">
+      <c r="A2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="23" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="26.25">
-      <c r="A3" s="27" t="s">
+    <row r="3" spans="1:3">
+      <c r="A3" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:3" s="24" customFormat="1">
+      <c r="A4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="29">
+      <c r="B4" s="25">
         <f>SUM(B3:B3)</f>
         <v>0</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4" s="25">
         <f>SUM(C3:C3)</f>
         <v>0</v>
       </c>
@@ -1653,29 +1696,30 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="41.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.7109375" style="29" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="29" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="C1" s="23" t="s">
         <v>56</v>
-      </c>
-      <c r="C1" s="26" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1684,7 +1728,7 @@
   <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A21"/>
+      <selection activeCell="A2" sqref="A2:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1693,100 +1737,100 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="20" customFormat="1" ht="12.75">
+      <c r="A2" s="27"/>
+    </row>
+    <row r="3" spans="1:1" s="20" customFormat="1" ht="12.75">
+      <c r="A3" s="27" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75">
-      <c r="A2" s="30"/>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="13" t="s">
+    <row r="4" spans="1:1" s="20" customFormat="1" ht="12.75">
+      <c r="A4" s="28" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
-      <c r="A4" s="31" t="s">
+    <row r="5" spans="1:1" s="20" customFormat="1" ht="12.75">
+      <c r="A5" s="28" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="31" t="s">
+    <row r="6" spans="1:1" s="20" customFormat="1" ht="12.75">
+      <c r="A6" s="28" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="31" t="s">
+    <row r="7" spans="1:1" s="20" customFormat="1" ht="12.75">
+      <c r="A7" s="28" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="31" t="s">
+    <row r="8" spans="1:1" s="20" customFormat="1" ht="12.75">
+      <c r="A8" s="28" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="31" t="s">
+    <row r="9" spans="1:1" s="20" customFormat="1" ht="12.75">
+      <c r="A9" s="28" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="31" t="s">
+    <row r="10" spans="1:1" s="20" customFormat="1" ht="12.75">
+      <c r="A10" s="28"/>
+    </row>
+    <row r="11" spans="1:1" s="20" customFormat="1" ht="25.5">
+      <c r="A11" s="28" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="32"/>
-    </row>
-    <row r="11" spans="1:1" ht="45">
-      <c r="A11" s="32" t="s">
+    <row r="12" spans="1:1" s="20" customFormat="1" ht="12.75">
+      <c r="A12" s="28"/>
+    </row>
+    <row r="13" spans="1:1" s="20" customFormat="1" ht="12.75">
+      <c r="A13" s="28" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="32"/>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="32" t="s">
+    <row r="14" spans="1:1" s="20" customFormat="1" ht="12.75">
+      <c r="A14" s="28" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
-      <c r="A14" s="31" t="s">
+    <row r="15" spans="1:1" s="20" customFormat="1" ht="25.5">
+      <c r="A15" s="28" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="30">
-      <c r="A15" s="31" t="s">
+    <row r="16" spans="1:1" s="20" customFormat="1" ht="38.25">
+      <c r="A16" s="28" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="45">
-      <c r="A16" s="31" t="s">
+    <row r="17" spans="1:1" s="20" customFormat="1" ht="38.25">
+      <c r="A17" s="28" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="45">
-      <c r="A17" s="31" t="s">
+    <row r="18" spans="1:1" s="20" customFormat="1" ht="25.5">
+      <c r="A18" s="28" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="30">
-      <c r="A18" s="31" t="s">
+    <row r="19" spans="1:1" s="20" customFormat="1" ht="25.5">
+      <c r="A19" s="28" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="30">
-      <c r="A19" s="31" t="s">
+    <row r="20" spans="1:1" s="20" customFormat="1" ht="12.75">
+      <c r="A20" s="28"/>
+    </row>
+    <row r="21" spans="1:1" s="20" customFormat="1" ht="12.75">
+      <c r="A21" s="28" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="32"/>
-    </row>
-    <row r="21" spans="1:1" ht="30">
-      <c r="A21" s="32" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TRANSLATE-485: XLS fix and documentation
</commit_message>
<xml_diff>
--- a/application/modules/editor/Plugins/SegmentStatistics/templates/export-template.xlsx
+++ b/application/modules/editor/Plugins/SegmentStatistics/templates/export-template.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="99">
   <si>
     <t>zu bereinigen (Zeitpunkt: Import, nicht gesperrte Segmente)</t>
   </si>
@@ -212,30 +212,6 @@
   </si>
   <si>
     <t>(6) Nacharbeit</t>
-  </si>
-  <si>
-    <t>Termini Status X: Anzahl der Termini in Segmenten, die den Status X haben (gezählt werden für den roten Block die rot markierten Termini, für den blauen Block die blau markierten)</t>
-  </si>
-  <si>
-    <t>Zeichen: werden immer im Target (Zielsprache) gezählt</t>
-  </si>
-  <si>
-    <t>Zeilen: Berechnung: Zeichen / 55</t>
-  </si>
-  <si>
-    <t>Termini im blauen Block: Termini im Source (Quellsprache) mit Entsprechung im Target (Zielsprache), im Editor blau markiert ( = termFound im source)</t>
-  </si>
-  <si>
-    <t>Segmente im roten Block: Segmente im Source (Quellsprache) mit mindestens einem rot markierten Terminus. Im Editor sind das zum Zeitpunkt des Imports alle nicht gesperrten Segmente (= segmentsNotFound im source)</t>
-  </si>
-  <si>
-    <t>Segmente im blauen Block: Segmente im Source (Quellsprache) mit mindestens einem blau markierten Terminus. Im Editor sind das alle gesperrten Segmente und ein Teil der nicht gesperrten (= segmentsFound im source)</t>
-  </si>
-  <si>
-    <t>Wörter im roten Block: Anzahl der Wörter in Segmenten mit mindestens einem rot markierten Terminus</t>
-  </si>
-  <si>
-    <t>Wörter im blauen Block: Anzahl der Wörter in Segmenten mit mindestens einem blau markierten Terminus</t>
   </si>
   <si>
     <t>Die Arbeitsblätter 3 bis n sind nach den Zeilen auf dem Blatt „Zusammenfassung“ benannt.</t>
@@ -253,6 +229,102 @@
       </rPr>
       <t xml:space="preserve">[nach Häufigkeit korrekt geordnet] </t>
     </r>
+  </si>
+  <si>
+    <t>Generell:</t>
+  </si>
+  <si>
+    <t>Arbeitsblätter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definition roter Block: </t>
+  </si>
+  <si>
+    <t>Statistiken im roten Block: Termini im Source (Quellsprache) ohne Entsprechung im Target (Zielsprache) vorhanden, im Editor rot markiert ( = termNotFound im source)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Definition blauer Block: </t>
+  </si>
+  <si>
+    <t>Statistiken im blauen Block: Termini im Source (Quellsprache) mit Entsprechung im Target (Zielsprache) vorhanden, im Editor blau markiert ( = termFound im source)</t>
+  </si>
+  <si>
+    <t>Segmente mit roten und blauen Termini:</t>
+  </si>
+  <si>
+    <t>Segmente mit roten und blauen Termini werden daher im roten und blauen Block gezählt.</t>
+  </si>
+  <si>
+    <t>Filter:</t>
+  </si>
+  <si>
+    <t>Daten können auch gefiltert sein, dies erkennt man am Zusatz filtered im Dateinamen. Alle Zahlen beziehen sich auf Segmente die dem Filter entsprechen.</t>
+  </si>
+  <si>
+    <t>Einzelne Spalten</t>
+  </si>
+  <si>
+    <t>Die Spalten Beschreibungen gelten jeweils analog für die gleichnamigen Spalten im blauen bzw. roten Block und für Export bzw. Import Daten.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segmente / Datei: </t>
+  </si>
+  <si>
+    <t>Gesamtanzahlt der Segmente in der Datei.</t>
+  </si>
+  <si>
+    <t>Zeichen:</t>
+  </si>
+  <si>
+    <t>werden immer im Target (Zielsprache) gezählt</t>
+  </si>
+  <si>
+    <t>Zeilen:</t>
+  </si>
+  <si>
+    <t>Berechnung: Zeichen / 55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Termini: </t>
+  </si>
+  <si>
+    <t>Anzahl der Terme (rot oder blau, je nach Bereich) im Source (Quellsprache)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Segmente: </t>
+  </si>
+  <si>
+    <t>Segmente im roten Block haben im Source (Quellsprache) mindestens einen rot markierten Terminus. Im Editor sind das zum Zeitpunkt des Imports alle nicht gesperrten Segmente (= segmentsNotFound im source)</t>
+  </si>
+  <si>
+    <t>Segmente im blauen Block haben im Source (Quellsprache) mindestens einen blau markierten Terminus. Im Editor sind das alle gesperrten Segmente und ein Teil der nicht gesperrten (= segmentsFound im source)</t>
+  </si>
+  <si>
+    <t>Termini / Zeile:</t>
+  </si>
+  <si>
+    <t>Durchschnitt, berechnet sich aus Termini pro Zeile</t>
+  </si>
+  <si>
+    <t>Termini / Segment:</t>
+  </si>
+  <si>
+    <t>Durchschnitt, berechnet sich aus Termini pro Segment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wörter: </t>
+  </si>
+  <si>
+    <t>werden immer im Target (Zielsprache) gezählt, Wörter im roten Block: Anzahl der Wörter in Segmenten mit mindestens einem rot markierten Terminus im Source (Zielsprache)</t>
+  </si>
+  <si>
+    <t>werden immer im Target (Zielsprache) gezählt, Wörter im blauen Block: Anzahl der Wörter in Segmenten mit mindestens einem blau markierten Terminus im Source (Zielsprache)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wörter / Segment: </t>
+  </si>
+  <si>
+    <t>Durchschnitt, berechnet sich aus Wörter pro Segment</t>
   </si>
 </sst>
 </file>
@@ -349,13 +421,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -372,6 +437,14 @@
     <font>
       <b/>
       <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -435,7 +508,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -476,17 +549,13 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -509,6 +578,14 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -816,74 +893,74 @@
     <row r="1" spans="1:54">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="31" t="s">
+      <c r="C1" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31"/>
-      <c r="R1" s="31"/>
-      <c r="S1" s="32" t="s">
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="32"/>
-      <c r="U1" s="32"/>
-      <c r="V1" s="32"/>
-      <c r="W1" s="32"/>
-      <c r="X1" s="32"/>
-      <c r="Y1" s="32"/>
-      <c r="Z1" s="32"/>
-      <c r="AA1" s="32"/>
-      <c r="AB1" s="32"/>
-      <c r="AC1" s="32"/>
-      <c r="AD1" s="32"/>
-      <c r="AE1" s="32"/>
-      <c r="AF1" s="32"/>
-      <c r="AG1" s="33" t="s">
+      <c r="T1" s="30"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="30"/>
+      <c r="W1" s="30"/>
+      <c r="X1" s="30"/>
+      <c r="Y1" s="30"/>
+      <c r="Z1" s="30"/>
+      <c r="AA1" s="30"/>
+      <c r="AB1" s="30"/>
+      <c r="AC1" s="30"/>
+      <c r="AD1" s="30"/>
+      <c r="AE1" s="30"/>
+      <c r="AF1" s="30"/>
+      <c r="AG1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="AH1" s="33"/>
-      <c r="AI1" s="33"/>
-      <c r="AJ1" s="33"/>
-      <c r="AK1" s="33"/>
-      <c r="AL1" s="33"/>
-      <c r="AM1" s="33"/>
-      <c r="AN1" s="33"/>
-      <c r="AO1" s="33"/>
-      <c r="AP1" s="33"/>
-      <c r="AQ1" s="33"/>
-      <c r="AR1" s="33"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="31"/>
+      <c r="AL1" s="31"/>
+      <c r="AM1" s="31"/>
+      <c r="AN1" s="31"/>
+      <c r="AO1" s="31"/>
+      <c r="AP1" s="31"/>
+      <c r="AQ1" s="31"/>
+      <c r="AR1" s="31"/>
       <c r="AS1" s="2"/>
       <c r="AT1" s="2"/>
-      <c r="AU1" s="34" t="s">
+      <c r="AU1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="AV1" s="34"/>
-      <c r="AW1" s="34"/>
-      <c r="AX1" s="34"/>
-      <c r="AY1" s="34"/>
-      <c r="AZ1" s="34"/>
-      <c r="BA1" s="34"/>
-      <c r="BB1" s="34"/>
-    </row>
-    <row r="2" spans="1:54" s="22" customFormat="1" ht="25.5">
+      <c r="AV1" s="32"/>
+      <c r="AW1" s="32"/>
+      <c r="AX1" s="32"/>
+      <c r="AY1" s="32"/>
+      <c r="AZ1" s="32"/>
+      <c r="BA1" s="32"/>
+      <c r="BB1" s="32"/>
+    </row>
+    <row r="2" spans="1:54" s="21" customFormat="1" ht="25.5">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -904,7 +981,7 @@
       <c r="H2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="20" t="s">
         <v>13</v>
       </c>
       <c r="J2" s="3" t="s">
@@ -928,40 +1005,40 @@
       <c r="P2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" s="21" t="s">
+      <c r="Q2" s="20" t="s">
         <v>13</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="21" t="s">
+      <c r="S2" s="20" t="s">
         <v>7</v>
       </c>
       <c r="T2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U2" s="21" t="s">
+      <c r="U2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="V2" s="21" t="s">
+      <c r="V2" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="W2" s="21" t="s">
+      <c r="W2" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="X2" s="21" t="s">
+      <c r="X2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="Y2" s="21" t="s">
+      <c r="Y2" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="Z2" s="21" t="s">
+      <c r="Z2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="AA2" s="21" t="s">
+      <c r="AA2" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="AB2" s="21" t="s">
+      <c r="AB2" s="20" t="s">
         <v>10</v>
       </c>
       <c r="AC2" s="3" t="s">
@@ -970,40 +1047,40 @@
       <c r="AD2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AE2" s="21" t="s">
+      <c r="AE2" s="20" t="s">
         <v>13</v>
       </c>
       <c r="AF2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AG2" s="21" t="s">
+      <c r="AG2" s="20" t="s">
         <v>7</v>
       </c>
       <c r="AH2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="AI2" s="21" t="s">
+      <c r="AI2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="AJ2" s="21" t="s">
+      <c r="AJ2" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="AK2" s="21" t="s">
+      <c r="AK2" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="AL2" s="21" t="s">
+      <c r="AL2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="AM2" s="21" t="s">
+      <c r="AM2" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="AN2" s="21" t="s">
+      <c r="AN2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="AO2" s="21" t="s">
+      <c r="AO2" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="AP2" s="21" t="s">
+      <c r="AP2" s="20" t="s">
         <v>10</v>
       </c>
       <c r="AQ2" s="3" t="s">
@@ -1012,7 +1089,7 @@
       <c r="AR2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AS2" s="21" t="s">
+      <c r="AS2" s="20" t="s">
         <v>13</v>
       </c>
       <c r="AT2" s="3" t="s">
@@ -1231,7 +1308,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="4" spans="1:54" s="22" customFormat="1" ht="12.75">
+    <row r="4" spans="1:54" s="21" customFormat="1" ht="12.75">
       <c r="A4" s="4" t="s">
         <v>50</v>
       </c>
@@ -1644,21 +1721,21 @@
     <col min="3" max="3" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="24" customFormat="1">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:3" s="23" customFormat="1">
+      <c r="A1" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-    </row>
-    <row r="2" spans="1:3" s="24" customFormat="1">
-      <c r="A2" s="23" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+    </row>
+    <row r="2" spans="1:3" s="23" customFormat="1">
+      <c r="A2" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="22" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1673,15 +1750,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="24" customFormat="1">
+    <row r="4" spans="1:3" s="23" customFormat="1">
       <c r="A4" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="24">
         <f>SUM(B3:B3)</f>
         <v>0</v>
       </c>
-      <c r="C4" s="25">
+      <c r="C4" s="24">
         <f>SUM(C3:C3)</f>
         <v>0</v>
       </c>
@@ -1701,19 +1778,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="55.7109375" style="29" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" style="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="29" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="55.7109375" style="27" customWidth="1"/>
+    <col min="2" max="2" width="17.140625" style="27" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" s="23" t="s">
+      <c r="A1" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="22" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1725,112 +1802,216 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A21"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD21"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="82.140625" customWidth="1"/>
+    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="2" max="2" width="133.42578125" style="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:2" ht="15.75">
+      <c r="A1" s="33" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:1" s="20" customFormat="1" ht="12.75">
-      <c r="A2" s="27"/>
-    </row>
-    <row r="3" spans="1:1" s="20" customFormat="1" ht="12.75">
-      <c r="A3" s="27" t="s">
+    <row r="2" spans="1:2" s="27" customFormat="1" ht="12.75">
+      <c r="A2" s="25"/>
+      <c r="B2" s="19"/>
+    </row>
+    <row r="3" spans="1:2" s="27" customFormat="1" ht="12.75">
+      <c r="A3" s="25" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" s="20" customFormat="1" ht="12.75">
-      <c r="A4" s="28" t="s">
+      <c r="B3" s="19"/>
+    </row>
+    <row r="4" spans="1:2" s="27" customFormat="1" ht="12.75">
+      <c r="A4" s="26" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" s="20" customFormat="1" ht="12.75">
-      <c r="A5" s="28" t="s">
+      <c r="B4" s="19"/>
+    </row>
+    <row r="5" spans="1:2" s="27" customFormat="1" ht="12.75">
+      <c r="A5" s="26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" s="20" customFormat="1" ht="12.75">
-      <c r="A6" s="28" t="s">
+      <c r="B5" s="19"/>
+    </row>
+    <row r="6" spans="1:2" s="27" customFormat="1" ht="12.75">
+      <c r="A6" s="26" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" s="20" customFormat="1" ht="12.75">
-      <c r="A7" s="28" t="s">
+      <c r="B6" s="19"/>
+    </row>
+    <row r="7" spans="1:2" s="27" customFormat="1" ht="12.75">
+      <c r="A7" s="26" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" s="20" customFormat="1" ht="12.75">
-      <c r="A8" s="28" t="s">
+      <c r="B7" s="19"/>
+    </row>
+    <row r="8" spans="1:2" s="27" customFormat="1" ht="25.5">
+      <c r="A8" s="26" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" s="20" customFormat="1" ht="12.75">
-      <c r="A9" s="28" t="s">
+      <c r="B8" s="19"/>
+    </row>
+    <row r="9" spans="1:2" s="27" customFormat="1" ht="12.75">
+      <c r="A9" s="26" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" s="20" customFormat="1" ht="12.75">
-      <c r="A10" s="28"/>
-    </row>
-    <row r="11" spans="1:1" s="20" customFormat="1" ht="25.5">
-      <c r="A11" s="28" t="s">
+      <c r="B9" s="19"/>
+    </row>
+    <row r="10" spans="1:2" s="27" customFormat="1" ht="12.75">
+      <c r="A10" s="26"/>
+      <c r="B10" s="19"/>
+    </row>
+    <row r="11" spans="1:2" s="27" customFormat="1" ht="12.75">
+      <c r="A11" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="19"/>
+    </row>
+    <row r="12" spans="1:2" s="27" customFormat="1" ht="12.75">
+      <c r="A12" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12" s="19" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:1" s="20" customFormat="1" ht="12.75">
-      <c r="A12" s="28"/>
-    </row>
-    <row r="13" spans="1:1" s="20" customFormat="1" ht="12.75">
-      <c r="A13" s="28" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" s="20" customFormat="1" ht="12.75">
-      <c r="A14" s="28" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" s="20" customFormat="1" ht="25.5">
-      <c r="A15" s="28" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" s="20" customFormat="1" ht="38.25">
-      <c r="A16" s="28" t="s">
+    <row r="13" spans="1:2" s="27" customFormat="1" ht="12.75">
+      <c r="A13" s="27" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" s="20" customFormat="1" ht="38.25">
-      <c r="A17" s="28" t="s">
+      <c r="B13" s="19" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="1:1" s="20" customFormat="1" ht="25.5">
-      <c r="A18" s="28" t="s">
+    <row r="14" spans="1:2" s="27" customFormat="1" ht="12.75">
+      <c r="A14" s="27" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" s="20" customFormat="1" ht="25.5">
-      <c r="A19" s="28" t="s">
+      <c r="B14" s="19" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="20" spans="1:1" s="20" customFormat="1" ht="12.75">
-      <c r="A20" s="28"/>
-    </row>
-    <row r="21" spans="1:1" s="20" customFormat="1" ht="12.75">
-      <c r="A21" s="28" t="s">
+    <row r="15" spans="1:2" s="27" customFormat="1" ht="25.5">
+      <c r="A15" s="26" t="s">
         <v>73</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" s="27" customFormat="1" ht="12.75">
+      <c r="A16" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="27" customFormat="1" ht="12.75">
+      <c r="B17" s="19"/>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="19"/>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="19"/>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="36" t="s">
+        <v>85</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="36"/>
+      <c r="B25" s="19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="36" t="s">
+        <v>94</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="36"/>
+      <c r="B29" s="19" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TRANSLATE-620: add columns for number of chars and lines per file to statistics
</commit_message>
<xml_diff>
--- a/application/modules/editor/Plugins/SegmentStatistics/templates/export-template.xlsx
+++ b/application/modules/editor/Plugins/SegmentStatistics/templates/export-template.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="102">
   <si>
     <t>zu bereinigen (Zeitpunkt: Import, nicht gesperrte Segmente)</t>
   </si>
@@ -325,6 +325,15 @@
   </si>
   <si>
     <t>Durchschnitt, berechnet sich aus Wörter pro Segment</t>
+  </si>
+  <si>
+    <t>Zeichen / Datei</t>
+  </si>
+  <si>
+    <t>Zeilen / Datei</t>
+  </si>
+  <si>
+    <t>STAT.import.target.charCount</t>
   </si>
 </sst>
 </file>
@@ -508,7 +517,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -563,6 +572,15 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -578,14 +596,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -880,407 +890,416 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BB7"/>
+  <dimension ref="A1:BD7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="60.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="2" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54">
+    <row r="1" spans="1:56">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="29" t="s">
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="30" t="s">
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="R1" s="34"/>
+      <c r="S1" s="34"/>
+      <c r="T1" s="34"/>
+      <c r="U1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="30"/>
-      <c r="U1" s="30"/>
-      <c r="V1" s="30"/>
-      <c r="W1" s="30"/>
-      <c r="X1" s="30"/>
-      <c r="Y1" s="30"/>
-      <c r="Z1" s="30"/>
-      <c r="AA1" s="30"/>
-      <c r="AB1" s="30"/>
-      <c r="AC1" s="30"/>
-      <c r="AD1" s="30"/>
-      <c r="AE1" s="30"/>
-      <c r="AF1" s="30"/>
-      <c r="AG1" s="31" t="s">
+      <c r="V1" s="35"/>
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
+      <c r="AA1" s="35"/>
+      <c r="AB1" s="35"/>
+      <c r="AC1" s="35"/>
+      <c r="AD1" s="35"/>
+      <c r="AE1" s="35"/>
+      <c r="AF1" s="35"/>
+      <c r="AG1" s="35"/>
+      <c r="AH1" s="35"/>
+      <c r="AI1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="31"/>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="31"/>
-      <c r="AL1" s="31"/>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="31"/>
-      <c r="AO1" s="31"/>
-      <c r="AP1" s="31"/>
-      <c r="AQ1" s="31"/>
-      <c r="AR1" s="31"/>
-      <c r="AS1" s="2"/>
-      <c r="AT1" s="2"/>
-      <c r="AU1" s="32" t="s">
+      <c r="AJ1" s="36"/>
+      <c r="AK1" s="36"/>
+      <c r="AL1" s="36"/>
+      <c r="AM1" s="36"/>
+      <c r="AN1" s="36"/>
+      <c r="AO1" s="36"/>
+      <c r="AP1" s="36"/>
+      <c r="AQ1" s="36"/>
+      <c r="AR1" s="36"/>
+      <c r="AS1" s="36"/>
+      <c r="AT1" s="36"/>
+      <c r="AU1" s="2"/>
+      <c r="AV1" s="2"/>
+      <c r="AW1" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="AV1" s="32"/>
-      <c r="AW1" s="32"/>
-      <c r="AX1" s="32"/>
-      <c r="AY1" s="32"/>
-      <c r="AZ1" s="32"/>
-      <c r="BA1" s="32"/>
-      <c r="BB1" s="32"/>
-    </row>
-    <row r="2" spans="1:54" s="21" customFormat="1" ht="25.5">
+      <c r="AX1" s="37"/>
+      <c r="AY1" s="37"/>
+      <c r="AZ1" s="37"/>
+      <c r="BA1" s="37"/>
+      <c r="BB1" s="37"/>
+      <c r="BC1" s="37"/>
+      <c r="BD1" s="37"/>
+    </row>
+    <row r="2" spans="1:56" s="21" customFormat="1" ht="25.5">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="K2" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="O2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="Q2" s="20" t="s">
+      <c r="S2" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="20" t="s">
+      <c r="U2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="U2" s="20" t="s">
+      <c r="W2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="V2" s="20" t="s">
+      <c r="X2" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="W2" s="20" t="s">
+      <c r="Y2" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="X2" s="20" t="s">
+      <c r="Z2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="Y2" s="20" t="s">
+      <c r="AA2" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="Z2" s="20" t="s">
+      <c r="AB2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="AA2" s="20" t="s">
+      <c r="AC2" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="AB2" s="20" t="s">
+      <c r="AD2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AE2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AF2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AE2" s="20" t="s">
+      <c r="AG2" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AH2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AG2" s="20" t="s">
+      <c r="AI2" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AJ2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="AI2" s="20" t="s">
+      <c r="AK2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="AJ2" s="20" t="s">
+      <c r="AL2" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="AK2" s="20" t="s">
+      <c r="AM2" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="AL2" s="20" t="s">
+      <c r="AN2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="AM2" s="20" t="s">
+      <c r="AO2" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="AN2" s="20" t="s">
+      <c r="AP2" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="AO2" s="20" t="s">
+      <c r="AQ2" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="AP2" s="20" t="s">
+      <c r="AR2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="AQ2" s="3" t="s">
+      <c r="AS2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AR2" s="3" t="s">
+      <c r="AT2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="AS2" s="20" t="s">
+      <c r="AU2" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="AT2" s="3" t="s">
+      <c r="AV2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="AU2" s="3" t="s">
+      <c r="AW2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AV2" s="3" t="s">
+      <c r="AX2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="AW2" s="3" t="s">
+      <c r="AY2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="AX2" s="3" t="s">
+      <c r="AZ2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="AY2" s="3" t="s">
+      <c r="BA2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="AZ2" s="3" t="s">
+      <c r="BB2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="BA2" s="3" t="s">
+      <c r="BC2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="BB2" s="3" t="s">
+      <c r="BD2" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:54" s="19" customFormat="1" ht="12.75">
+    <row r="3" spans="1:56" s="19" customFormat="1" ht="12.75">
       <c r="A3" s="18" t="s">
         <v>21</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="18" t="s">
-        <v>23</v>
+      <c r="C3" s="32" t="s">
+        <v>101</v>
       </c>
       <c r="D3" s="16" t="e">
         <f>ROUND(C3/55,0)</f>
         <v>#VALUE!</v>
       </c>
       <c r="E3" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="16" t="e">
+        <f>ROUND(E3/55,0)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G3" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="H3" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="16" t="e">
-        <f>ROUND(E3/D3, 2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H3" s="16" t="e">
-        <f>ROUND(E3/F3, 2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="16" t="e">
+        <f>ROUND(G3/F3, 2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J3" s="16" t="e">
+        <f>ROUND(G3/H3, 2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K3" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="16" t="e">
-        <f>ROUND(I3/F3,2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="K3" s="18" t="s">
+      <c r="L3" s="16" t="e">
+        <f>ROUND(K3/H3,2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M3" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="16" t="e">
-        <f>ROUND(K3/55,0)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M3" s="18" t="s">
+      <c r="N3" s="16" t="e">
+        <f>ROUND(M3/55,0)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O3" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="N3" s="18" t="s">
+      <c r="P3" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="O3" s="16" t="e">
-        <f>ROUND(M3/L3, 2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P3" s="16" t="e">
-        <f>ROUND(M3/N3, 2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Q3" s="18" t="s">
+      <c r="Q3" s="16" t="e">
+        <f>ROUND(O3/N3, 2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R3" s="16" t="e">
+        <f>ROUND(O3/P3, 2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="S3" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="R3" s="16" t="e">
-        <f>ROUND(Q3/N3,2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="S3" s="18" t="s">
+      <c r="T3" s="16" t="e">
+        <f>ROUND(S3/P3,2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U3" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="T3" s="16" t="e">
-        <f>ROUND(S3/55,0)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="U3" s="18" t="s">
+      <c r="V3" s="16" t="e">
+        <f>ROUND(U3/55,0)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="W3" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="V3" s="17" t="s">
+      <c r="X3" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="W3" s="17" t="s">
+      <c r="Y3" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="X3" s="17" t="s">
+      <c r="Z3" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="Y3" s="17" t="s">
+      <c r="AA3" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="Z3" s="17" t="s">
+      <c r="AB3" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="AA3" s="17" t="s">
+      <c r="AC3" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="AB3" s="18" t="s">
+      <c r="AD3" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="AC3" s="16" t="e">
-        <f>ROUND(U3/T3, 2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AD3" s="16" t="e">
-        <f>ROUND(U3/AB3, 2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AE3" s="17" t="s">
+      <c r="AE3" s="16" t="e">
+        <f>ROUND(W3/V3, 2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AF3" s="16" t="e">
+        <f>ROUND(W3/AD3, 2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AG3" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="AF3" s="16" t="e">
-        <f>ROUND(AE3/AB3,2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AG3" s="18" t="s">
+      <c r="AH3" s="16" t="e">
+        <f>ROUND(AG3/AD3,2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AI3" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="AH3" s="16" t="e">
-        <f>ROUND(AG3/55,0)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AI3" s="18" t="s">
+      <c r="AJ3" s="16" t="e">
+        <f>ROUND(AI3/55,0)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AK3" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="AJ3" s="17" t="s">
+      <c r="AL3" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="AK3" s="17" t="s">
+      <c r="AM3" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="AL3" s="17" t="s">
+      <c r="AN3" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="AM3" s="17" t="s">
+      <c r="AO3" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="AN3" s="17" t="s">
+      <c r="AP3" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="AO3" s="17" t="s">
+      <c r="AQ3" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="AP3" s="18" t="s">
+      <c r="AR3" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="AQ3" s="16" t="e">
-        <f>ROUND(AI3/AH3, 2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AR3" s="16" t="e">
-        <f>ROUND(AI3/AP3, 2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AS3" s="17" t="s">
+      <c r="AS3" s="16" t="e">
+        <f>ROUND(AK3/AJ3, 2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AT3" s="16" t="e">
+        <f>ROUND(AK3/AR3, 2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AU3" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="AT3" s="16" t="e">
-        <f>ROUND(AS3/AP3,2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AU3" s="16" t="e">
-        <f>C3-S3</f>
-        <v>#VALUE!</v>
-      </c>
       <c r="AV3" s="16" t="e">
-        <f>D3-T3</f>
+        <f>ROUND(AU3/AR3,2)</f>
         <v>#VALUE!</v>
       </c>
       <c r="AW3" s="16" t="e">
@@ -1288,27 +1307,35 @@
         <v>#VALUE!</v>
       </c>
       <c r="AX3" s="16" t="e">
-        <f>F3-AB3</f>
+        <f>F3-V3</f>
         <v>#VALUE!</v>
       </c>
       <c r="AY3" s="16" t="e">
-        <f>ROUND(AW3/AV3, 2)</f>
+        <f>G3-W3</f>
         <v>#VALUE!</v>
       </c>
       <c r="AZ3" s="16" t="e">
-        <f>ROUND(AW3/AX3, 2)</f>
+        <f>H3-AD3</f>
         <v>#VALUE!</v>
       </c>
       <c r="BA3" s="16" t="e">
-        <f>I3-AE3</f>
+        <f>ROUND(AY3/AX3, 2)</f>
         <v>#VALUE!</v>
       </c>
       <c r="BB3" s="16" t="e">
-        <f>BA3/AX3</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="4" spans="1:54" s="21" customFormat="1" ht="12.75">
+        <f>ROUND(AY3/AZ3, 2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BC3" s="16" t="e">
+        <f>K3-AG3</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BD3" s="16" t="e">
+        <f>BC3/AZ3</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:56" s="21" customFormat="1" ht="12.75">
       <c r="A4" s="4" t="s">
         <v>50</v>
       </c>
@@ -1320,7 +1347,7 @@
         <f>SUM(C3:C3)</f>
         <v>0</v>
       </c>
-      <c r="D4" s="3" t="e">
+      <c r="D4" s="4" t="e">
         <f>SUM(D3:D3)</f>
         <v>#VALUE!</v>
       </c>
@@ -1328,73 +1355,73 @@
         <f>SUM(E3:E3)</f>
         <v>0</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3" t="e">
         <f>SUM(F3:F3)</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="3" t="e">
-        <f>ROUND(E4/D4, 2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H4" s="3" t="e">
-        <f t="shared" ref="H4" si="0">ROUND(E4/F4, 2)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I4" s="4">
-        <f>SUM(I3:I3)</f>
-        <v>0</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G4" s="4">
+        <f>SUM(G3:G3)</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="4">
+        <f>SUM(H3:H3)</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="3" t="e">
+        <f>ROUND(G4/F4, 2)</f>
+        <v>#VALUE!</v>
       </c>
       <c r="J4" s="3" t="e">
-        <f>ROUND(I4/F4,2)</f>
+        <f t="shared" ref="J4" si="0">ROUND(G4/H4, 2)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K4" s="4">
         <f>SUM(K3:K3)</f>
         <v>0</v>
       </c>
-      <c r="L4" s="4" t="e">
-        <f>SUM(L3:L3)</f>
-        <v>#VALUE!</v>
+      <c r="L4" s="3" t="e">
+        <f>ROUND(K4/H4,2)</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="M4" s="4">
         <f>SUM(M3:M3)</f>
         <v>0</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4" s="4" t="e">
         <f>SUM(N3:N3)</f>
-        <v>0</v>
-      </c>
-      <c r="O4" s="3" t="e">
-        <f>ROUND(M4/L4, 2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="P4" s="3" t="e">
-        <f t="shared" ref="P4" si="1">ROUND(M4/N4, 2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O4" s="4">
+        <f>SUM(O3:O3)</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="4">
+        <f>SUM(P3:P3)</f>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="3" t="e">
+        <f>ROUND(O4/N4, 2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R4" s="3" t="e">
+        <f t="shared" ref="R4" si="1">ROUND(O4/P4, 2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="Q4" s="4">
-        <f>SUM(Q3:Q3)</f>
-        <v>0</v>
-      </c>
-      <c r="R4" s="3" t="e">
-        <f>ROUND(Q4/N4,2)</f>
+      <c r="S4" s="4">
+        <f>SUM(S3:S3)</f>
+        <v>0</v>
+      </c>
+      <c r="T4" s="3" t="e">
+        <f>ROUND(S4/P4,2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="S4" s="4">
-        <f t="shared" ref="S4:AB4" si="2">SUM(S3:S3)</f>
-        <v>0</v>
-      </c>
-      <c r="T4" s="4" t="e">
+      <c r="U4" s="4">
+        <f t="shared" ref="U4:AD4" si="2">SUM(U3:U3)</f>
+        <v>0</v>
+      </c>
+      <c r="V4" s="4" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
-      </c>
-      <c r="U4" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="V4" s="4">
-        <f t="shared" si="2"/>
-        <v>0</v>
       </c>
       <c r="W4" s="4">
         <f t="shared" si="2"/>
@@ -1420,37 +1447,37 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AC4" s="3" t="e">
-        <f>ROUND(U4/T4, 2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AD4" s="3" t="e">
-        <f>ROUND(U4/AB4, 2)</f>
+      <c r="AC4" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AD4" s="4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AE4" s="3" t="e">
+        <f>ROUND(W4/V4, 2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AF4" s="3" t="e">
+        <f>ROUND(W4/AD4, 2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AE4" s="4">
-        <f>SUM(AE3:AE3)</f>
-        <v>0</v>
-      </c>
-      <c r="AF4" s="3" t="e">
-        <f>ROUND(AE4/AB4,2)</f>
+      <c r="AG4" s="4">
+        <f>SUM(AG3:AG3)</f>
+        <v>0</v>
+      </c>
+      <c r="AH4" s="3" t="e">
+        <f>ROUND(AG4/AD4,2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AG4" s="4">
-        <f t="shared" ref="AG4:AP4" si="3">SUM(AG3:AG3)</f>
-        <v>0</v>
-      </c>
-      <c r="AH4" s="4" t="e">
+      <c r="AI4" s="4">
+        <f t="shared" ref="AI4:AR4" si="3">SUM(AI3:AI3)</f>
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="4" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
-      </c>
-      <c r="AI4" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AJ4" s="4">
-        <f t="shared" si="3"/>
-        <v>0</v>
       </c>
       <c r="AK4" s="4">
         <f t="shared" si="3"/>
@@ -1476,32 +1503,32 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="AQ4" s="3" t="e">
-        <f>ROUND(AI4/AH4, 2)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AR4" s="3" t="e">
-        <f>ROUND(AI4/AP4, 2)</f>
+      <c r="AQ4" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AR4" s="4">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AS4" s="3" t="e">
+        <f>ROUND(AK4/AJ4, 2)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="AT4" s="3" t="e">
+        <f>ROUND(AK4/AR4, 2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AS4" s="4">
-        <f>SUM(AS3:AS3)</f>
-        <v>0</v>
-      </c>
-      <c r="AT4" s="3" t="e">
-        <f>ROUND(AS4/AP4,2)</f>
+      <c r="AU4" s="4">
+        <f>SUM(AU3:AU3)</f>
+        <v>0</v>
+      </c>
+      <c r="AV4" s="3" t="e">
+        <f>ROUND(AU4/AR4,2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="AU4" s="4" t="e">
-        <f t="shared" ref="AU4:BB4" si="4">SUM(AU3:AU3)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="AV4" s="4" t="e">
-        <f t="shared" si="4"/>
-        <v>#VALUE!</v>
-      </c>
       <c r="AW4" s="4" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="AW4:BD4" si="4">SUM(AW3:AW3)</f>
         <v>#VALUE!</v>
       </c>
       <c r="AX4" s="4" t="e">
@@ -1524,17 +1551,25 @@
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="5" spans="1:54">
+      <c r="BC4" s="4" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="BD4" s="4" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:56">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="7"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
       <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="8"/>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
@@ -1544,53 +1579,55 @@
       <c r="P5" s="9"/>
       <c r="Q5" s="9"/>
       <c r="R5" s="9"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="11"/>
+      <c r="S5" s="9"/>
+      <c r="T5" s="9"/>
       <c r="U5" s="10"/>
-      <c r="V5" s="10"/>
+      <c r="V5" s="11"/>
       <c r="W5" s="10"/>
       <c r="X5" s="10"/>
       <c r="Y5" s="10"/>
       <c r="Z5" s="10"/>
       <c r="AA5" s="10"/>
       <c r="AB5" s="10"/>
-      <c r="AC5" s="11"/>
+      <c r="AC5" s="10"/>
       <c r="AD5" s="10"/>
-      <c r="AE5" s="10"/>
+      <c r="AE5" s="11"/>
       <c r="AF5" s="10"/>
-      <c r="AG5" s="12"/>
-      <c r="AH5" s="11"/>
+      <c r="AG5" s="10"/>
+      <c r="AH5" s="10"/>
       <c r="AI5" s="12"/>
-      <c r="AJ5" s="12"/>
+      <c r="AJ5" s="11"/>
       <c r="AK5" s="12"/>
       <c r="AL5" s="12"/>
       <c r="AM5" s="12"/>
       <c r="AN5" s="12"/>
       <c r="AO5" s="12"/>
       <c r="AP5" s="12"/>
-      <c r="AQ5" s="11"/>
-      <c r="AR5" s="10"/>
-      <c r="AS5" s="10"/>
+      <c r="AQ5" s="12"/>
+      <c r="AR5" s="12"/>
+      <c r="AS5" s="11"/>
       <c r="AT5" s="10"/>
-      <c r="AU5" s="12"/>
-      <c r="AV5" s="11"/>
+      <c r="AU5" s="10"/>
+      <c r="AV5" s="10"/>
       <c r="AW5" s="12"/>
-      <c r="AX5" s="12"/>
-      <c r="AY5" s="11"/>
-      <c r="AZ5" s="11"/>
+      <c r="AX5" s="11"/>
+      <c r="AY5" s="12"/>
+      <c r="AZ5" s="12"/>
       <c r="BA5" s="11"/>
-      <c r="BB5" s="9"/>
-    </row>
-    <row r="6" spans="1:54">
+      <c r="BB5" s="11"/>
+      <c r="BC5" s="11"/>
+      <c r="BD5" s="9"/>
+    </row>
+    <row r="6" spans="1:56">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
       <c r="C6" s="12"/>
-      <c r="D6" s="11"/>
+      <c r="D6" s="12"/>
       <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="11"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
@@ -1600,55 +1637,57 @@
       <c r="P6" s="9"/>
       <c r="Q6" s="9"/>
       <c r="R6" s="9"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="11"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
       <c r="U6" s="10"/>
-      <c r="V6" s="10"/>
+      <c r="V6" s="11"/>
       <c r="W6" s="10"/>
       <c r="X6" s="10"/>
       <c r="Y6" s="10"/>
       <c r="Z6" s="10"/>
       <c r="AA6" s="10"/>
       <c r="AB6" s="10"/>
-      <c r="AC6" s="11"/>
+      <c r="AC6" s="10"/>
       <c r="AD6" s="10"/>
-      <c r="AE6" s="10"/>
+      <c r="AE6" s="11"/>
       <c r="AF6" s="10"/>
-      <c r="AG6" s="12"/>
-      <c r="AH6" s="11"/>
+      <c r="AG6" s="10"/>
+      <c r="AH6" s="10"/>
       <c r="AI6" s="12"/>
-      <c r="AJ6" s="12"/>
+      <c r="AJ6" s="11"/>
       <c r="AK6" s="12"/>
       <c r="AL6" s="12"/>
       <c r="AM6" s="12"/>
       <c r="AN6" s="12"/>
       <c r="AO6" s="12"/>
       <c r="AP6" s="12"/>
-      <c r="AQ6" s="11"/>
-      <c r="AR6" s="10"/>
-      <c r="AS6" s="10"/>
+      <c r="AQ6" s="12"/>
+      <c r="AR6" s="12"/>
+      <c r="AS6" s="11"/>
       <c r="AT6" s="10"/>
-      <c r="AU6" s="12"/>
-      <c r="AV6" s="11"/>
+      <c r="AU6" s="10"/>
+      <c r="AV6" s="10"/>
       <c r="AW6" s="12"/>
-      <c r="AX6" s="12"/>
-      <c r="AY6" s="11"/>
-      <c r="AZ6" s="11"/>
+      <c r="AX6" s="11"/>
+      <c r="AY6" s="12"/>
+      <c r="AZ6" s="12"/>
       <c r="BA6" s="11"/>
-      <c r="BB6" s="9"/>
-    </row>
-    <row r="7" spans="1:54">
+      <c r="BB6" s="11"/>
+      <c r="BC6" s="11"/>
+      <c r="BD6" s="9"/>
+    </row>
+    <row r="7" spans="1:56">
       <c r="A7" s="13" t="s">
         <v>51</v>
       </c>
       <c r="B7" s="13"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="11"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
       <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="11"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
@@ -1658,50 +1697,52 @@
       <c r="P7" s="9"/>
       <c r="Q7" s="9"/>
       <c r="R7" s="9"/>
-      <c r="S7" s="10"/>
-      <c r="T7" s="11"/>
+      <c r="S7" s="9"/>
+      <c r="T7" s="9"/>
       <c r="U7" s="10"/>
-      <c r="V7" s="10"/>
+      <c r="V7" s="11"/>
       <c r="W7" s="10"/>
       <c r="X7" s="10"/>
       <c r="Y7" s="10"/>
       <c r="Z7" s="10"/>
       <c r="AA7" s="10"/>
       <c r="AB7" s="10"/>
-      <c r="AC7" s="11"/>
+      <c r="AC7" s="10"/>
       <c r="AD7" s="10"/>
-      <c r="AE7" s="10"/>
+      <c r="AE7" s="11"/>
       <c r="AF7" s="10"/>
-      <c r="AG7" s="12"/>
-      <c r="AH7" s="11"/>
+      <c r="AG7" s="10"/>
+      <c r="AH7" s="10"/>
       <c r="AI7" s="12"/>
-      <c r="AJ7" s="12"/>
+      <c r="AJ7" s="11"/>
       <c r="AK7" s="12"/>
       <c r="AL7" s="12"/>
       <c r="AM7" s="12"/>
       <c r="AN7" s="12"/>
       <c r="AO7" s="12"/>
       <c r="AP7" s="12"/>
-      <c r="AQ7" s="11"/>
-      <c r="AR7" s="10"/>
-      <c r="AS7" s="10"/>
+      <c r="AQ7" s="12"/>
+      <c r="AR7" s="12"/>
+      <c r="AS7" s="11"/>
       <c r="AT7" s="10"/>
-      <c r="AU7" s="12"/>
-      <c r="AV7" s="11"/>
+      <c r="AU7" s="10"/>
+      <c r="AV7" s="10"/>
       <c r="AW7" s="12"/>
-      <c r="AX7" s="12"/>
-      <c r="AY7" s="11"/>
-      <c r="AZ7" s="11"/>
+      <c r="AX7" s="11"/>
+      <c r="AY7" s="12"/>
+      <c r="AZ7" s="12"/>
       <c r="BA7" s="11"/>
-      <c r="BB7" s="9"/>
+      <c r="BB7" s="11"/>
+      <c r="BC7" s="11"/>
+      <c r="BD7" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="C1:J1"/>
-    <mergeCell ref="K1:R1"/>
-    <mergeCell ref="S1:AF1"/>
-    <mergeCell ref="AG1:AR1"/>
-    <mergeCell ref="AU1:BB1"/>
+    <mergeCell ref="E1:L1"/>
+    <mergeCell ref="M1:T1"/>
+    <mergeCell ref="U1:AH1"/>
+    <mergeCell ref="AI1:AT1"/>
+    <mergeCell ref="AW1:BD1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1811,11 +1852,11 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="133.42578125" style="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="133.42578125" style="29" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.75">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="28" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1870,7 +1911,7 @@
       <c r="B10" s="19"/>
     </row>
     <row r="11" spans="1:2" s="27" customFormat="1" ht="12.75">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="30" t="s">
         <v>67</v>
       </c>
       <c r="B11" s="19"/>
@@ -1919,7 +1960,7 @@
       <c r="B17" s="19"/>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="35" t="s">
+      <c r="A18" s="30" t="s">
         <v>77</v>
       </c>
       <c r="B18" s="19"/>
@@ -1931,7 +1972,7 @@
       <c r="B19" s="19"/>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="31" t="s">
         <v>79</v>
       </c>
       <c r="B20" s="19" t="s">
@@ -1939,7 +1980,7 @@
       </c>
     </row>
     <row r="21" spans="1:2">
-      <c r="A21" s="36" t="s">
+      <c r="A21" s="31" t="s">
         <v>81</v>
       </c>
       <c r="B21" s="19" t="s">
@@ -1947,7 +1988,7 @@
       </c>
     </row>
     <row r="22" spans="1:2">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="31" t="s">
         <v>83</v>
       </c>
       <c r="B22" s="19" t="s">
@@ -1955,7 +1996,7 @@
       </c>
     </row>
     <row r="23" spans="1:2">
-      <c r="A23" s="36" t="s">
+      <c r="A23" s="31" t="s">
         <v>85</v>
       </c>
       <c r="B23" s="19" t="s">
@@ -1963,7 +2004,7 @@
       </c>
     </row>
     <row r="24" spans="1:2">
-      <c r="A24" s="36" t="s">
+      <c r="A24" s="31" t="s">
         <v>87</v>
       </c>
       <c r="B24" s="19" t="s">
@@ -1971,13 +2012,13 @@
       </c>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="36"/>
+      <c r="A25" s="31"/>
       <c r="B25" s="19" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="36" t="s">
+      <c r="A26" s="31" t="s">
         <v>90</v>
       </c>
       <c r="B26" s="19" t="s">
@@ -1985,7 +2026,7 @@
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="31" t="s">
         <v>92</v>
       </c>
       <c r="B27" s="19" t="s">
@@ -1993,7 +2034,7 @@
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="31" t="s">
         <v>94</v>
       </c>
       <c r="B28" s="19" t="s">
@@ -2001,13 +2042,13 @@
       </c>
     </row>
     <row r="29" spans="1:2">
-      <c r="A29" s="36"/>
+      <c r="A29" s="31"/>
       <c r="B29" s="19" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="36" t="s">
+      <c r="A30" s="31" t="s">
         <v>97</v>
       </c>
       <c r="B30" s="19" t="s">

</xml_diff>